<commit_message>
Changed declaration in ExcelutiilityFile
</commit_message>
<xml_diff>
--- a/src/test/resources/SkillraryTestdata.xlsx
+++ b/src/test/resources/SkillraryTestdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16680" windowHeight="6540"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16380" windowHeight="6540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Wanted Brouchure for the course and details</t>
+    <t xml:space="preserve">Wanted Brouchure </t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>